<commit_message>
8.22 test for web
</commit_message>
<xml_diff>
--- a/result/rnn-test11.xlsx
+++ b/result/rnn-test11.xlsx
@@ -423,13 +423,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.9419999999999999</v>
+        <v>0.9485791610284168</v>
       </c>
       <c r="C2">
-        <v>0.9651639344262295</v>
+        <v>0.9576502732240437</v>
       </c>
       <c r="D2">
-        <v>0.9534412955465587</v>
+        <v>0.9530931339225017</v>
       </c>
       <c r="E2">
         <v>1464</v>
@@ -440,13 +440,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.966</v>
+        <v>0.9592641261498029</v>
       </c>
       <c r="C3">
-        <v>0.943359375</v>
+        <v>0.9505208333333334</v>
       </c>
       <c r="D3">
-        <v>0.9545454545454545</v>
+        <v>0.9548724656638327</v>
       </c>
       <c r="E3">
         <v>1536</v>
@@ -474,13 +474,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.954</v>
+        <v>0.9539216435891098</v>
       </c>
       <c r="C5">
-        <v>0.9542616547131147</v>
+        <v>0.9540855532786885</v>
       </c>
       <c r="D5">
-        <v>0.9539933750460066</v>
+        <v>0.9539827997931671</v>
       </c>
       <c r="E5">
         <v>3000</v>
@@ -491,13 +491,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.9542879999999999</v>
+        <v>0.9540498631705665</v>
       </c>
       <c r="C6">
         <v>0.954</v>
       </c>
       <c r="D6">
-        <v>0.9540066249539932</v>
+        <v>0.9540041517740632</v>
       </c>
       <c r="E6">
         <v>3000</v>

</xml_diff>